<commit_message>
Piccole aggiunte al file Datasource
</commit_message>
<xml_diff>
--- a/Solution/PptGeneratorGUI/DataSourceFolder/Info.xlsx
+++ b/Solution/PptGeneratorGUI/DataSourceFolder/Info.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\Lefo\Dev\3 GDPptGenerator\Solution\PptGeneratorGUI\DataSourceFolder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F859E99-80FB-4FAA-882C-896A6E51D977}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79B1A889-BB29-441B-9C7E-ADC9080122CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6000" yWindow="6300" windowWidth="28800" windowHeight="15225" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4230" yWindow="4080" windowWidth="28800" windowHeight="15225" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Formule-Budget" sheetId="3" r:id="rId1"/>
@@ -503,7 +503,7 @@
   <dimension ref="A2:C31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12:B23"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>